<commit_message>
add MLP model and fix MLModels Config
</commit_message>
<xml_diff>
--- a/data/output/KPIs_all_features.xlsx
+++ b/data/output/KPIs_all_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Vie Professionnelle\CDI Dec 2024 - Data Scientist\Entretiens\Quod_Financial\Quod_THA\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2394B48A-4C89-40FC-932C-ED47DEF8D552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A120A2B-5817-40C9-80EF-F28A75E1FCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yearly" sheetId="1" r:id="rId1"/>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>